<commit_message>
Added extOpStats statistics function
</commit_message>
<xml_diff>
--- a/Power/Uinput.xlsx
+++ b/Power/Uinput.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Malik B\Documents\Research\dataset\MATLab Code\Functions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniil\Documents\ORS_2016\MATLAB\Power\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>Minimun useful voltage of the system? (V)</t>
-  </si>
-  <si>
-    <t>Test.txt</t>
   </si>
   <si>
     <r>
@@ -121,11 +118,14 @@
   <si>
     <t xml:space="preserve">How Many cycles to predict consecutivley? </t>
   </si>
+  <si>
+    <t>SetupA.txt</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -448,28 +448,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="52" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="1"/>
+    <col min="5" max="5" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -477,20 +477,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -498,7 +498,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -506,39 +506,39 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="E10" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -546,12 +546,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -559,7 +559,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -567,7 +567,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -575,42 +575,42 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="1">
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" s="1">
         <f>(B17*B18)/60</f>
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>24</v>
       </c>
       <c r="B20" s="1">
         <v>10</v>

</xml_diff>